<commit_message>
Further timing experiment results
</commit_message>
<xml_diff>
--- a/Resources/Timing results.xlsx
+++ b/Resources/Timing results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>New Year's eve commit</t>
   </si>
@@ -34,12 +34,21 @@
   </si>
   <si>
     <t>slack /ns</t>
+  </si>
+  <si>
+    <t>Reduce to 16 V M's</t>
+  </si>
+  <si>
+    <t>Shrink Sstack and reduce to 16VM's</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,12 +86,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,15 +394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -462,7 +472,7 @@
       <c r="I2">
         <v>90</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>0.01</v>
       </c>
       <c r="K2">
@@ -482,7 +492,7 @@
       <c r="C3">
         <v>34</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3">
@@ -502,6 +512,82 @@
       </c>
       <c r="J3">
         <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E4">
+        <v>73</v>
+      </c>
+      <c r="F4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I4">
+        <v>43</v>
+      </c>
+      <c r="J4">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E5">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="G5">
+        <v>54</v>
+      </c>
+      <c r="H5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I5">
+        <v>95</v>
+      </c>
+      <c r="J5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K5">
+        <v>45</v>
+      </c>
+      <c r="L5">
+        <v>2.4E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>